<commit_message>
fillit: first successful solution, more tests needed
</commit_message>
<xml_diff>
--- a/fillit/tetrim.xlsx
+++ b/fillit/tetrim.xlsx
@@ -424,11 +424,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -444,53 +442,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
+      <c r="A1" s="4">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4">
+        <v>3</v>
+      </c>
       <c r="E1" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F1" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G1" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H1" s="4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I1" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J1" s="4">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K1" s="8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="L1" s="4">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="M1" s="4">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="N1" s="4">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="O1" s="8">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="P1" s="4">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="4">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="R1" s="4">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="S1" s="8">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="T1" s="4">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -1790,6 +1800,84 @@
       </c>
       <c r="T23" s="5">
         <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20">
+      <c r="B25" s="4">
+        <f>SUM(B3:B23)</f>
+        <v>6</v>
+      </c>
+      <c r="C25" s="4">
+        <f t="shared" ref="C25:T25" si="0">SUM(C3:C23)</f>
+        <v>6</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H25" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I25" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J25" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K25" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L25" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M25" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="N25" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="O25" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="P25" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Q25" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="R25" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="S25" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="T25" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>